<commit_message>
Added an ELISA pipeline
</commit_message>
<xml_diff>
--- a/ReadME_Template.xlsx
+++ b/ReadME_Template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20399"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E470385-8377-4930-9130-D77108C2E881}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A99797A-3C08-485D-8DD4-CCFB5B32133C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Tabs</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Above Fit Curve Range</t>
   </si>
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
     <t>Identification of assay, plates and operators</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
     <t>Total # of plates</t>
   </si>
   <si>
-    <t>Plate #1 assay</t>
-  </si>
-  <si>
     <t>Plate #1 ID</t>
   </si>
   <si>
@@ -70,24 +61,6 @@
     <t>Plate #1 run date</t>
   </si>
   <si>
-    <t>Plate #2 assay</t>
-  </si>
-  <si>
-    <t>Plate #2 ID</t>
-  </si>
-  <si>
-    <t>Plate #2 run date</t>
-  </si>
-  <si>
-    <t>Plate #3 assay</t>
-  </si>
-  <si>
-    <t>Plate #3 ID</t>
-  </si>
-  <si>
-    <t>Plate #3 run date</t>
-  </si>
-  <si>
     <t>pg/mL</t>
   </si>
   <si>
@@ -109,30 +82,15 @@
     <t>Dilution summary</t>
   </si>
   <si>
-    <t>Dilution BALF samples</t>
-  </si>
-  <si>
-    <t>Dilution QC_1_1_22</t>
-  </si>
-  <si>
     <t>Freeze/thaw summary</t>
   </si>
   <si>
     <t>Freeze/thaws samples</t>
   </si>
   <si>
-    <t>Freeze/ thaw QC_1_1_22</t>
-  </si>
-  <si>
     <t xml:space="preserve">ask for how QC was named </t>
   </si>
   <si>
-    <t>Antibody Lots</t>
-  </si>
-  <si>
-    <t>Plate ID</t>
-  </si>
-  <si>
     <t>WideData</t>
   </si>
   <si>
@@ -224,6 +182,18 @@
   </si>
   <si>
     <t>Units of Measure</t>
+  </si>
+  <si>
+    <t>Assay</t>
+  </si>
+  <si>
+    <t>Dilution Samples/QC</t>
+  </si>
+  <si>
+    <t>Plate Assays</t>
+  </si>
+  <si>
+    <t>Freeze/thaw QC_1_1_22</t>
   </si>
 </sst>
 </file>
@@ -231,7 +201,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -267,13 +237,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,27 +261,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,405 +560,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="105.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="7" t="s">
+    </row>
+    <row r="10" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    </row>
+    <row r="20" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8" t="s">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    </row>
+    <row r="25" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    </row>
+    <row r="28" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    </row>
+    <row r="29" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    </row>
+    <row r="30" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    </row>
+    <row r="31" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="10"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="8"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="34" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="5">
+        <v>-89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="5">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="8"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="13"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+    </row>
+    <row r="42" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="13"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="13"/>
-    </row>
-    <row r="55" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="14">
-        <v>-99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="14">
-        <v>-89</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B60" s="4"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B62" s="5"/>
+      <c r="B43" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>